<commit_message>
update the time display
</commit_message>
<xml_diff>
--- a/Customer_data.xlsx
+++ b/Customer_data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,32 +563,72 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>13:14:15 PM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>200987643V</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>06/07/2023</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>11.45</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>thellmbura</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0771249582</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>200987643V</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>06/07/2023</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>11.45</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>thellmbura</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0771249582</t>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>r</t>
         </is>
       </c>
     </row>

</xml_diff>